<commit_message>
updated virus.txt and varroa-virus. rmd
</commit_message>
<xml_diff>
--- a/23_viruses_mapping.xlsx
+++ b/23_viruses_mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nuriteliash/Documents/GitHub/varroa-virus-networks/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nuriteliash/OneDrive - OIST/Repos/varroa-virus-networks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9AA001-10E2-0849-9EF3-A6ACEE9A60A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{AD9AA001-10E2-0849-9EF3-A6ACEE9A60A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A7E8609C-FFAD-2747-B883-C4AF896D9156}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" xr2:uid="{CF879805-FEE3-454F-A828-3042F3F81762}"/>
   </bookViews>
@@ -263,9 +263,6 @@
     <t>﻿Mordecai (2016)</t>
   </si>
   <si>
-    <t>﻿ERS657949</t>
-  </si>
-  <si>
     <t>Deformed wing virus type c</t>
   </si>
   <si>
@@ -390,6 +387,9 @@
   </si>
   <si>
     <t>VDV1</t>
+  </si>
+  <si>
+    <t>ENA|CEND01000001|CEND01000001.1</t>
   </si>
 </sst>
 </file>
@@ -978,14 +978,14 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="37.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="37.83203125" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" style="3" customWidth="1"/>
@@ -995,7 +995,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="18" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>88</v>
@@ -1004,24 +1004,24 @@
         <v>87</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="15" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>81</v>
@@ -1036,7 +1036,7 @@
         <v>10140</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>27</v>
@@ -1047,12 +1047,12 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" t="s">
         <v>77</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="15" t="s">
         <v>76</v>
       </c>
       <c r="D3" t="s">
@@ -1073,13 +1073,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
         <v>74</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>73</v>
-      </c>
-      <c r="C4" t="s">
-        <v>72</v>
       </c>
       <c r="D4" t="s">
         <v>71</v>
@@ -1099,13 +1099,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
         <v>69</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>68</v>
-      </c>
-      <c r="C5" t="s">
-        <v>67</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -1125,13 +1125,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="C6" t="s">
-        <v>63</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
@@ -1151,13 +1151,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
         <v>61</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>59</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
@@ -1177,13 +1177,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
         <v>57</v>
-      </c>
-      <c r="C8" t="s">
-        <v>56</v>
       </c>
       <c r="D8" t="s">
         <v>20</v>
@@ -1203,13 +1203,13 @@
     </row>
     <row r="9" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="C9" t="s">
-        <v>52</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
@@ -1229,13 +1229,13 @@
     </row>
     <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
         <v>50</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>48</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>
@@ -1255,13 +1255,13 @@
     </row>
     <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
         <v>46</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>44</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
@@ -1281,13 +1281,13 @@
     </row>
     <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" t="s">
         <v>42</v>
-      </c>
-      <c r="C12" t="s">
-        <v>41</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -1307,13 +1307,13 @@
     </row>
     <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
@@ -1333,13 +1333,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
@@ -1359,13 +1359,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
       </c>
       <c r="D15" t="s">
         <v>20</v>
@@ -1385,13 +1385,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="C16" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="C16" t="s">
-        <v>24</v>
       </c>
       <c r="D16" t="s">
         <v>20</v>
@@ -1411,13 +1411,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="C17" t="s">
-        <v>21</v>
       </c>
       <c r="D17" t="s">
         <v>20</v>
@@ -1437,13 +1437,13 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="C18" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
       </c>
       <c r="D18" t="s">
         <v>16</v>
@@ -1463,13 +1463,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -1489,13 +1489,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="C20" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
       </c>
       <c r="D20" t="s">
         <v>3</v>
@@ -1515,13 +1515,13 @@
     </row>
     <row r="21" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="C21" s="23" t="s">
         <v>5</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>4</v>
       </c>
       <c r="D21" s="22" t="s">
         <v>3</v>
@@ -1541,13 +1541,13 @@
     </row>
     <row r="22" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="28" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="D22" s="25" t="s">
         <v>20</v>
@@ -1556,7 +1556,7 @@
         <v>6169</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G22" s="29" t="s">
         <v>27</v>
@@ -1567,13 +1567,13 @@
     </row>
     <row r="23" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="28" t="s">
         <v>93</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>95</v>
       </c>
       <c r="D23" s="32" t="s">
         <v>16</v>
@@ -1582,7 +1582,7 @@
         <v>8332</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G23" s="34" t="s">
         <v>1</v>
@@ -1592,14 +1592,14 @@
       </c>
     </row>
     <row r="24" spans="1:8" s="38" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" s="37" t="s">
+      <c r="A24" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="C24" s="38" t="s">
-        <v>103</v>
+      <c r="C24" s="37" t="s">
+        <v>104</v>
       </c>
       <c r="D24" s="16" t="s">
         <v>20</v>
@@ -1608,7 +1608,7 @@
         <v>2198</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G24" s="40" t="s">
         <v>1</v>
@@ -1618,14 +1618,14 @@
       </c>
     </row>
     <row r="25" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>104</v>
+      <c r="A25" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>111</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>20</v>
@@ -1634,7 +1634,7 @@
         <v>1899</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G25" s="29" t="s">
         <v>1</v>
@@ -1644,14 +1644,14 @@
       </c>
     </row>
     <row r="26" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>102</v>
+      <c r="A26" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>112</v>
       </c>
       <c r="D26" s="25" t="s">
         <v>20</v>
@@ -1660,7 +1660,7 @@
         <v>1983</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G26" s="29" t="s">
         <v>1</v>
@@ -1670,14 +1670,14 @@
       </c>
     </row>
     <row r="27" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="B27" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="C27" s="31" t="s">
-        <v>101</v>
+      <c r="A27" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>113</v>
       </c>
       <c r="D27" s="25" t="s">
         <v>20</v>
@@ -1686,7 +1686,7 @@
         <v>1708</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G27" s="29" t="s">
         <v>1</v>
@@ -1696,14 +1696,14 @@
       </c>
     </row>
     <row r="28" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="B28" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>100</v>
+      <c r="A28" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>114</v>
       </c>
       <c r="D28" s="25" t="s">
         <v>20</v>
@@ -1712,7 +1712,7 @@
         <v>1442</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G28" s="29" t="s">
         <v>1</v>
@@ -1722,14 +1722,14 @@
       </c>
     </row>
     <row r="29" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="B29" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="C29" s="46" t="s">
-        <v>99</v>
+      <c r="A29" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" s="45" t="s">
+        <v>115</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>20</v>
@@ -1738,7 +1738,7 @@
         <v>951</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G29" s="47" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
update virus.txt to match SRRs (virus names)
</commit_message>
<xml_diff>
--- a/23_viruses_mapping.xlsx
+++ b/23_viruses_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nuriteliash/OneDrive - OIST/Repos/varroa-virus-networks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{AD9AA001-10E2-0849-9EF3-A6ACEE9A60A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A7E8609C-FFAD-2747-B883-C4AF896D9156}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{AD9AA001-10E2-0849-9EF3-A6ACEE9A60A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E03E2066-51E4-2945-BA8E-8CA1268FF9E8}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" xr2:uid="{CF879805-FEE3-454F-A828-3042F3F81762}"/>
   </bookViews>
@@ -71,9 +71,6 @@
     <t>dsDNA</t>
   </si>
   <si>
-    <t>﻿KR819915</t>
-  </si>
-  <si>
     <t>﻿Apis mellifera Filamentous virus (AmFV)</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>De miranda (2015)</t>
   </si>
   <si>
-    <t xml:space="preserve"> NC_027631.1 </t>
-  </si>
-  <si>
     <t>Bee Macula-like virus isolate France 878V, complete genome</t>
   </si>
   <si>
@@ -329,24 +323,6 @@
     <t>VTLV</t>
   </si>
   <si>
-    <t>MK032470</t>
-  </si>
-  <si>
-    <t>MK032469</t>
-  </si>
-  <si>
-    <t>MK032468</t>
-  </si>
-  <si>
-    <t>MK032467</t>
-  </si>
-  <si>
-    <t xml:space="preserve">﻿MK032465     </t>
-  </si>
-  <si>
-    <t>MK032466</t>
-  </si>
-  <si>
     <t>Varroa orthomyxovirus-1 isolate IL segment 1</t>
   </si>
   <si>
@@ -390,6 +366,30 @@
   </si>
   <si>
     <t>ENA|CEND01000001|CEND01000001.1</t>
+  </si>
+  <si>
+    <t>MK032466.1</t>
+  </si>
+  <si>
+    <t>MK032467.1</t>
+  </si>
+  <si>
+    <t>MK032468.1</t>
+  </si>
+  <si>
+    <t>MK032469.1</t>
+  </si>
+  <si>
+    <t>MK032470.1</t>
+  </si>
+  <si>
+    <t>﻿KR819915.1</t>
+  </si>
+  <si>
+    <t>﻿MK032465.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC_027631.1 </t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -532,42 +532,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -640,7 +609,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -650,9 +618,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -661,6 +627,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -978,13 +945,13 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="22" customWidth="1"/>
     <col min="3" max="3" width="37.83203125" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" customWidth="1"/>
@@ -994,153 +961,153 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="18" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>88</v>
-      </c>
       <c r="C1" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="15" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>81</v>
-      </c>
       <c r="C2" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="17">
         <v>10140</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" t="s">
-        <v>77</v>
+      <c r="A3" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>75</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3">
         <v>10169</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B4" t="s">
-        <v>74</v>
-      </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E4" s="6">
         <v>9499</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="6">
         <v>9524</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B6" t="s">
-        <v>65</v>
-      </c>
       <c r="C6" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="6">
         <v>3674</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>0</v>
@@ -1150,75 +1117,75 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B7" t="s">
-        <v>61</v>
-      </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="6">
         <v>9491</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" t="s">
-        <v>89</v>
+      <c r="A8" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="6">
         <v>9505</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
       <c r="C9" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="6">
         <v>5991</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>0</v>
@@ -1228,49 +1195,49 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B10" t="s">
-        <v>50</v>
-      </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="6">
         <v>8550</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10" s="13" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B11" t="s">
-        <v>46</v>
-      </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="6">
         <v>8832</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>1</v>
@@ -1280,127 +1247,127 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" t="s">
-        <v>117</v>
+      <c r="A12" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>109</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="6">
         <v>10112</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H12" s="13" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
       <c r="C13" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="6">
         <v>9552</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="B14" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
       <c r="C14" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>0</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" s="6">
         <v>6258</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>25</v>
-      </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" s="6">
         <v>20414</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>1</v>
@@ -1410,23 +1377,23 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="6">
         <v>10091</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>1</v>
@@ -1436,23 +1403,23 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>18</v>
-      </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" s="6">
         <v>14001</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>1</v>
@@ -1462,14 +1429,14 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -1488,10 +1455,10 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="22" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1541,100 +1508,100 @@
     </row>
     <row r="22" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="28" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E22" s="25">
         <v>6169</v>
       </c>
       <c r="F22" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G22" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="G22" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="H22" s="30" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>93</v>
-      </c>
       <c r="D23" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E23" s="33">
         <v>8332</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G23" s="34" t="s">
         <v>1</v>
       </c>
       <c r="H23" s="35" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="38" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="B24" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="C24" s="37" t="s">
-        <v>104</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>96</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="39">
+        <v>19</v>
+      </c>
+      <c r="E24" s="38">
         <v>2198</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="G24" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="H24" s="41" t="s">
+      <c r="H24" s="40" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="B25" s="42" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>111</v>
-      </c>
       <c r="D25" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="43">
+        <v>19</v>
+      </c>
+      <c r="E25" s="41">
         <v>1899</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G25" s="29" t="s">
         <v>1</v>
@@ -1645,22 +1612,22 @@
     </row>
     <row r="26" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26" s="42" t="s">
-        <v>107</v>
+        <v>112</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>99</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="43">
+        <v>19</v>
+      </c>
+      <c r="E26" s="41">
         <v>1983</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G26" s="29" t="s">
         <v>1</v>
@@ -1671,48 +1638,48 @@
     </row>
     <row r="27" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="B27" s="42" t="s">
-        <v>108</v>
-      </c>
       <c r="C27" s="28" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="43">
+        <v>19</v>
+      </c>
+      <c r="E27" s="41">
         <v>1708</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G27" s="29" t="s">
         <v>1</v>
       </c>
       <c r="H27" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="B28" s="42" t="s">
-        <v>109</v>
+        <v>114</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>101</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" s="43">
+        <v>19</v>
+      </c>
+      <c r="E28" s="41">
         <v>1442</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G28" s="29" t="s">
         <v>1</v>
@@ -1721,29 +1688,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="B29" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="C29" s="45" t="s">
+    <row r="29" spans="1:8" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="31" t="s">
         <v>115</v>
       </c>
+      <c r="B29" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="42" t="s">
+        <v>107</v>
+      </c>
       <c r="D29" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" s="46">
+        <v>19</v>
+      </c>
+      <c r="E29" s="43">
         <v>951</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G29" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="G29" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="H29" s="48" t="s">
+      <c r="H29" s="45" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
varroa modules and interactions with virus
</commit_message>
<xml_diff>
--- a/23_viruses_mapping.xlsx
+++ b/23_viruses_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nuriteliash/OneDrive - OIST/Repos/varroa-virus-networks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{AD9AA001-10E2-0849-9EF3-A6ACEE9A60A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E03E2066-51E4-2945-BA8E-8CA1268FF9E8}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{AD9AA001-10E2-0849-9EF3-A6ACEE9A60A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E2873A2D-6010-1C43-A3EC-C632083F9D83}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" xr2:uid="{CF879805-FEE3-454F-A828-3042F3F81762}"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="28800" windowHeight="16000" xr2:uid="{CF879805-FEE3-454F-A828-3042F3F81762}"/>
   </bookViews>
   <sheets>
     <sheet name="for mapping" sheetId="1" r:id="rId1"/>
@@ -396,7 +396,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -452,6 +452,20 @@
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -536,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -584,15 +598,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -628,6 +634,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -944,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB62654-CEDF-844B-8E52-83ECC4F9D602}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -961,10 +987,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="18" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="42" t="s">
         <v>86</v>
       </c>
       <c r="C1" s="18" t="s">
@@ -1090,29 +1116,29 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
+    <row r="6" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="6">
+      <c r="D6" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="46">
         <v>3674</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4" t="s">
+      <c r="G6" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="49" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1350,55 +1376,55 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="22" t="s">
+    <row r="16" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="6">
+      <c r="D16" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="46">
         <v>20414</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="22" t="s">
+      <c r="H16" s="49" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="D17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="6">
+      <c r="D17" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="46">
         <v>10091</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="49" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1454,263 +1480,263 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
+    <row r="20" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="46">
         <v>1811</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="22" t="s">
+      <c r="H20" s="49" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="24">
+      <c r="E21" s="51">
         <v>2194</v>
       </c>
-      <c r="F21" s="25" t="s">
+      <c r="F21" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="G21" s="26" t="s">
+      <c r="G21" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="H21" s="27" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="28" t="s">
+      <c r="H21" s="54" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="25">
+      <c r="D22" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="23">
         <v>6169</v>
       </c>
-      <c r="F22" s="25" t="s">
+      <c r="F22" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="G22" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22" s="30" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
+      <c r="G22" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="33">
+      <c r="E23" s="29">
         <v>8332</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G23" s="34" t="s">
+      <c r="G23" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="H23" s="35" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="H23" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="33" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="32" t="s">
         <v>96</v>
       </c>
       <c r="D24" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="38">
+      <c r="E24" s="34">
         <v>2198</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="G24" s="39" t="s">
+      <c r="G24" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="H24" s="40" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="31" t="s">
+      <c r="H24" s="36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="D25" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="41">
+      <c r="D25" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="37">
         <v>1899</v>
       </c>
-      <c r="F25" s="25" t="s">
+      <c r="F25" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="G25" s="29" t="s">
+      <c r="G25" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H25" s="30" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="31" t="s">
+      <c r="H25" s="26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="41">
+      <c r="D26" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="37">
         <v>1983</v>
       </c>
-      <c r="F26" s="25" t="s">
+      <c r="F26" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="G26" s="29" t="s">
+      <c r="G26" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H26" s="30" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="31" t="s">
+      <c r="H26" s="26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="D27" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="41">
+      <c r="D27" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="37">
         <v>1708</v>
       </c>
-      <c r="F27" s="25" t="s">
+      <c r="F27" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="G27" s="29" t="s">
+      <c r="G27" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H27" s="30" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="31" t="s">
+      <c r="H27" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="D28" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="41">
+      <c r="D28" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="37">
         <v>1442</v>
       </c>
-      <c r="F28" s="25" t="s">
+      <c r="F28" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="G28" s="29" t="s">
+      <c r="G28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H28" s="30" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="43" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="31" t="s">
+      <c r="H28" s="26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="38" t="s">
         <v>107</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="43">
+      <c r="E29" s="39">
         <v>951</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G29" s="44" t="s">
+      <c r="G29" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="H29" s="45" t="s">
+      <c r="H29" s="41" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>